<commit_message>
Add tidy page to survey data
</commit_message>
<xml_diff>
--- a/messy-project-directory/data/survey_data.xlsx
+++ b/messy-project-directory/data/survey_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineramossarmiento/Downloads/tfcb-homework01/messy-project-directory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C88D94-0454-3D43-8448-219BEB599A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="19640" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="tidy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="45">
   <si>
     <t>NA</t>
   </si>
@@ -140,14 +141,39 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t>Date_Collected</t>
+  </si>
+  <si>
+    <t>Weight(g)</t>
+  </si>
+  <si>
+    <t>Field_Season</t>
+  </si>
+  <si>
+    <t>Scale_Calibrated</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>OL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -162,11 +188,13 @@
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="28"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
@@ -177,11 +205,13 @@
       <b/>
       <sz val="24"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
@@ -334,12 +364,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +830,7 @@
   <dimension ref="C3:AB28"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="M8" sqref="M8:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -903,294 +933,294 @@
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1229,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1410,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E33" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -2286,4 +2316,1146 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B85F6E-C9FC-3D40-AA24-15E42564D700}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="21">
+        <v>41471</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2013</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="21">
+        <v>41471</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2013</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="21">
+        <v>41471</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2013</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="21">
+        <v>41471</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2013</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="21">
+        <v>41473</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2013</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="21">
+        <v>41473</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2013</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="21">
+        <v>41473</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2013</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="21">
+        <v>41473</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2013</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="21">
+        <v>41505</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>2013</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="21">
+        <v>41564</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>2013</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="21">
+        <v>41564</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12">
+        <v>2013</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="21">
+        <v>41618</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>2013</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="21">
+        <v>41618</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14">
+        <v>2013</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="21">
+        <v>41619</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15">
+        <v>2013</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="21">
+        <v>41590</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>2013</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>126</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>2013</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>2013</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>113</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>2013</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>122</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>2013</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>107</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>2013</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="21">
+        <v>41591</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>2013</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="21">
+        <v>41648</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>2014</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="21">
+        <v>41648</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2014</v>
+      </c>
+      <c r="G24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="21">
+        <v>41711</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2014</v>
+      </c>
+      <c r="G25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="21">
+        <v>41711</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>2014</v>
+      </c>
+      <c r="G26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="21">
+        <v>41711</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>146</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>2014</v>
+      </c>
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>2014</v>
+      </c>
+      <c r="G28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2014</v>
+      </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>2014</v>
+      </c>
+      <c r="G30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>2014</v>
+      </c>
+      <c r="G31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <v>2014</v>
+      </c>
+      <c r="G32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>157</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>2014</v>
+      </c>
+      <c r="G33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="21">
+        <v>41647</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>2014</v>
+      </c>
+      <c r="G34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="21">
+        <v>41688</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>218</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>2014</v>
+      </c>
+      <c r="G35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="21">
+        <v>41688</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>2014</v>
+      </c>
+      <c r="G36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="21">
+        <v>41688</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>2014</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="21">
+        <v>42074</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>2014</v>
+      </c>
+      <c r="G38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="21">
+        <v>42102</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>2014</v>
+      </c>
+      <c r="G39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="21">
+        <v>42130</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40">
+        <v>2014</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="21">
+        <v>42142</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>182</v>
+      </c>
+      <c r="E41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>2014</v>
+      </c>
+      <c r="G41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="21">
+        <v>42164</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>29</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>2014</v>
+      </c>
+      <c r="G42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="21">
+        <v>42193</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>115</v>
+      </c>
+      <c r="E43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>2014</v>
+      </c>
+      <c r="G43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="21">
+        <v>42193</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>190</v>
+      </c>
+      <c r="E44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>2014</v>
+      </c>
+      <c r="G44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45" s="21">
+        <v>28498</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>2014</v>
+      </c>
+      <c r="G45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46" s="21">
+        <v>28498</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>2014</v>
+      </c>
+      <c r="G46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="21">
+        <v>28498</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>48</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>2014</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="21">
+        <v>28498</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>52</v>
+      </c>
+      <c r="E48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48">
+        <v>2014</v>
+      </c>
+      <c r="G48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49" s="21">
+        <v>28498</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>35</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49">
+        <v>2014</v>
+      </c>
+      <c r="G49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>